<commit_message>
fix wrapping and heights
</commit_message>
<xml_diff>
--- a/src/ExcelsiorAspose.Tests/ComplexTypeWithCustomRender.Test.verified.xlsx
+++ b/src/ExcelsiorAspose.Tests/ComplexTypeWithCustomRender.Test.verified.xlsx
@@ -74,7 +74,7 @@
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -471,11 +471,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="8.71428571428571" customWidth="1"/>
+    <col min="1" max="1" width="9.71428571428571" customWidth="1"/>
     <col min="2" max="2" width="35.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="13" customHeight="1">
+    <row r="1" spans="1:2" ht="14" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -483,7 +483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="13" customHeight="1">
+    <row r="2" spans="1:2" ht="14" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>